<commit_message>
Fixed invalid links in Excel Domain Renderer
</commit_message>
<xml_diff>
--- a/docs/Simple/Simple Example.xlsx
+++ b/docs/Simple/Simple Example.xlsx
@@ -669,7 +669,7 @@
         <v>53</v>
       </c>
       <c r="B2" s="0">
-        <f>VLOOKUP(A2,Группы!A:B,2,0)</f>
+        <f>VLOOKUP(A2,'Группы'!A:B,2,0)</f>
       </c>
       <c r="C2" t="s" s="0">
         <v>56</v>
@@ -695,7 +695,7 @@
         <v>75</v>
       </c>
       <c r="B3" s="0">
-        <f>VLOOKUP(A3,Группы!A:B,2,0)</f>
+        <f>VLOOKUP(A3,'Группы'!A:B,2,0)</f>
       </c>
       <c r="C3" t="s" s="0">
         <v>77</v>
@@ -721,7 +721,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="0">
-        <f>VLOOKUP(A4,Группы!A:B,2,0)</f>
+        <f>VLOOKUP(A4,'Группы'!A:B,2,0)</f>
       </c>
       <c r="C4" t="s" s="0">
         <v>97</v>
@@ -747,7 +747,7 @@
         <v>75</v>
       </c>
       <c r="B5" s="0">
-        <f>VLOOKUP(A5,Группы!A:B,2,0)</f>
+        <f>VLOOKUP(A5,'Группы'!A:B,2,0)</f>
       </c>
       <c r="C5" t="s" s="0">
         <v>104</v>
@@ -848,7 +848,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="0">
-        <f>VLOOKUP(B2,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B2,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D2" t="s" s="0">
         <v>60</v>
@@ -895,7 +895,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="0">
-        <f>VLOOKUP(B3,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B3,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D3" t="s" s="0">
         <v>60</v>
@@ -942,7 +942,7 @@
         <v>77</v>
       </c>
       <c r="C4" s="0">
-        <f>VLOOKUP(B4,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B4,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D4" t="s" s="0">
         <v>60</v>
@@ -995,7 +995,7 @@
         <v>77</v>
       </c>
       <c r="C5" s="0">
-        <f>VLOOKUP(B5,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B5,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D5" t="s" s="0">
         <v>60</v>
@@ -1042,7 +1042,7 @@
         <v>77</v>
       </c>
       <c r="C6" s="0">
-        <f>VLOOKUP(B6,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B6,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D6" t="s" s="0">
         <v>60</v>
@@ -1089,7 +1089,7 @@
         <v>77</v>
       </c>
       <c r="C7" s="0">
-        <f>VLOOKUP(B7,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B7,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D7" t="s" s="0">
         <v>92</v>
@@ -1139,7 +1139,7 @@
         <v>97</v>
       </c>
       <c r="C8" s="0">
-        <f>VLOOKUP(B8,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B8,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D8" t="s" s="0">
         <v>60</v>
@@ -1192,7 +1192,7 @@
         <v>97</v>
       </c>
       <c r="C9" s="0">
-        <f>VLOOKUP(B9,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B9,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D9" t="s" s="0">
         <v>60</v>
@@ -1239,7 +1239,7 @@
         <v>97</v>
       </c>
       <c r="C10" s="0">
-        <f>VLOOKUP(B10,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B10,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D10" t="s" s="0">
         <v>92</v>
@@ -1289,7 +1289,7 @@
         <v>104</v>
       </c>
       <c r="C11" s="0">
-        <f>VLOOKUP(B11,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B11,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D11" t="s" s="0">
         <v>60</v>
@@ -1339,7 +1339,7 @@
         <v>104</v>
       </c>
       <c r="C12" s="0">
-        <f>VLOOKUP(B12,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B12,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D12" t="s" s="0">
         <v>60</v>
@@ -1389,7 +1389,7 @@
         <v>104</v>
       </c>
       <c r="C13" s="0">
-        <f>VLOOKUP(B13,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B13,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D13" t="s" s="0">
         <v>60</v>
@@ -1439,7 +1439,7 @@
         <v>104</v>
       </c>
       <c r="C14" s="0">
-        <f>VLOOKUP(B14,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B14,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D14" t="s" s="0">
         <v>92</v>
@@ -1525,7 +1525,7 @@
         <v>77</v>
       </c>
       <c r="C2" s="0">
-        <f>VLOOKUP(B2,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B2,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D2" t="s" s="0">
         <v>94</v>
@@ -1545,7 +1545,7 @@
         <v>104</v>
       </c>
       <c r="C3" s="0">
-        <f>VLOOKUP(B3,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B3,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D3" t="s" s="0">
         <v>113</v>
@@ -1601,22 +1601,22 @@
         <v>96</v>
       </c>
       <c r="B2" s="0">
-        <f>VLOOKUP(A2,Индексы!A:E,2,0)</f>
+        <f>VLOOKUP(A2,'Индексы'!A:E,2,0)</f>
       </c>
       <c r="C2" s="0">
-        <f>VLOOKUP(A2,Индексы!A:E,3,0)</f>
+        <f>VLOOKUP(A2,'Индексы'!A:E,3,0)</f>
       </c>
       <c r="D2" s="0">
-        <f>VLOOKUP(A2,Индексы!A:E,4,0)</f>
+        <f>VLOOKUP(A2,'Индексы'!A:E,4,0)</f>
       </c>
       <c r="E2" s="0">
-        <f>VLOOKUP(A2,Индексы!A:E,5,0)</f>
+        <f>VLOOKUP(A2,'Индексы'!A:E,5,0)</f>
       </c>
       <c r="F2" t="s" s="0">
         <v>90</v>
       </c>
       <c r="G2" s="0">
-        <f>VLOOKUP(B2&amp;"."&amp;F2,Поля таблиц!A:G,7,0)</f>
+        <f>VLOOKUP(B2&amp;"."&amp;F2,'Поля таблиц'!A:G,7,0)</f>
       </c>
     </row>
     <row r="3">
@@ -1624,22 +1624,22 @@
         <v>96</v>
       </c>
       <c r="B3" s="0">
-        <f>VLOOKUP(A3,Индексы!A:E,2,0)</f>
+        <f>VLOOKUP(A3,'Индексы'!A:E,2,0)</f>
       </c>
       <c r="C3" s="0">
-        <f>VLOOKUP(A3,Индексы!A:E,3,0)</f>
+        <f>VLOOKUP(A3,'Индексы'!A:E,3,0)</f>
       </c>
       <c r="D3" s="0">
-        <f>VLOOKUP(A3,Индексы!A:E,4,0)</f>
+        <f>VLOOKUP(A3,'Индексы'!A:E,4,0)</f>
       </c>
       <c r="E3" s="0">
-        <f>VLOOKUP(A3,Индексы!A:E,5,0)</f>
+        <f>VLOOKUP(A3,'Индексы'!A:E,5,0)</f>
       </c>
       <c r="F3" t="s" s="0">
         <v>87</v>
       </c>
       <c r="G3" s="0">
-        <f>VLOOKUP(B3&amp;"."&amp;F3,Поля таблиц!A:G,7,0)</f>
+        <f>VLOOKUP(B3&amp;"."&amp;F3,'Поля таблиц'!A:G,7,0)</f>
       </c>
     </row>
     <row r="4">
@@ -1647,22 +1647,22 @@
         <v>115</v>
       </c>
       <c r="B4" s="0">
-        <f>VLOOKUP(A4,Индексы!A:E,2,0)</f>
+        <f>VLOOKUP(A4,'Индексы'!A:E,2,0)</f>
       </c>
       <c r="C4" s="0">
-        <f>VLOOKUP(A4,Индексы!A:E,3,0)</f>
+        <f>VLOOKUP(A4,'Индексы'!A:E,3,0)</f>
       </c>
       <c r="D4" s="0">
-        <f>VLOOKUP(A4,Индексы!A:E,4,0)</f>
+        <f>VLOOKUP(A4,'Индексы'!A:E,4,0)</f>
       </c>
       <c r="E4" s="0">
-        <f>VLOOKUP(A4,Индексы!A:E,5,0)</f>
+        <f>VLOOKUP(A4,'Индексы'!A:E,5,0)</f>
       </c>
       <c r="F4" t="s" s="0">
         <v>109</v>
       </c>
       <c r="G4" s="0">
-        <f>VLOOKUP(B4&amp;"."&amp;F4,Поля таблиц!A:G,7,0)</f>
+        <f>VLOOKUP(B4&amp;"."&amp;F4,'Поля таблиц'!A:G,7,0)</f>
       </c>
     </row>
     <row r="5">
@@ -1670,22 +1670,22 @@
         <v>115</v>
       </c>
       <c r="B5" s="0">
-        <f>VLOOKUP(A5,Индексы!A:E,2,0)</f>
+        <f>VLOOKUP(A5,'Индексы'!A:E,2,0)</f>
       </c>
       <c r="C5" s="0">
-        <f>VLOOKUP(A5,Индексы!A:E,3,0)</f>
+        <f>VLOOKUP(A5,'Индексы'!A:E,3,0)</f>
       </c>
       <c r="D5" s="0">
-        <f>VLOOKUP(A5,Индексы!A:E,4,0)</f>
+        <f>VLOOKUP(A5,'Индексы'!A:E,4,0)</f>
       </c>
       <c r="E5" s="0">
-        <f>VLOOKUP(A5,Индексы!A:E,5,0)</f>
+        <f>VLOOKUP(A5,'Индексы'!A:E,5,0)</f>
       </c>
       <c r="F5" t="s" s="0">
         <v>111</v>
       </c>
       <c r="G5" s="0">
-        <f>VLOOKUP(B5&amp;"."&amp;F5,Поля таблиц!A:G,7,0)</f>
+        <f>VLOOKUP(B5&amp;"."&amp;F5,'Поля таблиц'!A:G,7,0)</f>
       </c>
     </row>
   </sheetData>
@@ -1744,7 +1744,7 @@
         <v>104</v>
       </c>
       <c r="C2" s="0">
-        <f>VLOOKUP(B2,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B2,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D2" t="s" s="0">
         <v>109</v>
@@ -1759,7 +1759,7 @@
         <v>97</v>
       </c>
       <c r="H2" s="0">
-        <f>VLOOKUP(G2,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(G2,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="I2" t="s" s="0">
         <v>118</v>
@@ -1779,7 +1779,7 @@
         <v>104</v>
       </c>
       <c r="C3" s="0">
-        <f>VLOOKUP(B3,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(B3,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="D3" t="s" s="0">
         <v>111</v>
@@ -1794,7 +1794,7 @@
         <v>77</v>
       </c>
       <c r="H3" s="0">
-        <f>VLOOKUP(G3,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(G3,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="I3" t="s" s="0">
         <v>118</v>
@@ -1859,34 +1859,34 @@
         <v>119</v>
       </c>
       <c r="B2" s="0">
-        <f>VLOOKUP(A2,Отношения!A:E,2,0)</f>
+        <f>VLOOKUP(A2,'Отношения'!A:E,2,0)</f>
       </c>
       <c r="C2" s="0">
-        <f>VLOOKUP(A2,Отношения!A:E,3,0)</f>
+        <f>VLOOKUP(A2,'Отношения'!A:E,3,0)</f>
       </c>
       <c r="D2" t="s" s="0">
         <v>97</v>
       </c>
       <c r="E2" s="0">
-        <f>VLOOKUP(D2,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(D2,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="F2" s="0">
-        <f>VLOOKUP(A2,Отношения!A:E,4,0)</f>
+        <f>VLOOKUP(A2,'Отношения'!A:E,4,0)</f>
       </c>
       <c r="G2" s="0">
-        <f>VLOOKUP(A2,Отношения!A:E,5,0)</f>
+        <f>VLOOKUP(A2,'Отношения'!A:E,5,0)</f>
       </c>
       <c r="H2" t="s" s="0">
         <v>109</v>
       </c>
       <c r="I2" s="0">
-        <f>VLOOKUP(B2&amp;"."&amp;H2,Поля таблиц!A:G,7,0)</f>
+        <f>VLOOKUP(B2&amp;"."&amp;H2,'Поля таблиц'!A:G,7,0)</f>
       </c>
       <c r="J2" t="s" s="0">
         <v>81</v>
       </c>
       <c r="K2" s="0">
-        <f>VLOOKUP(D2&amp;"."&amp;J2,Поля таблиц!A:G,7,0)</f>
+        <f>VLOOKUP(D2&amp;"."&amp;J2,'Поля таблиц'!A:G,7,0)</f>
       </c>
     </row>
     <row r="3">
@@ -1894,34 +1894,34 @@
         <v>121</v>
       </c>
       <c r="B3" s="0">
-        <f>VLOOKUP(A3,Отношения!A:E,2,0)</f>
+        <f>VLOOKUP(A3,'Отношения'!A:E,2,0)</f>
       </c>
       <c r="C3" s="0">
-        <f>VLOOKUP(A3,Отношения!A:E,3,0)</f>
+        <f>VLOOKUP(A3,'Отношения'!A:E,3,0)</f>
       </c>
       <c r="D3" t="s" s="0">
         <v>77</v>
       </c>
       <c r="E3" s="0">
-        <f>VLOOKUP(D3,Таблицы!C:D,2,0)</f>
+        <f>VLOOKUP(D3,'Таблицы'!C:D,2,0)</f>
       </c>
       <c r="F3" s="0">
-        <f>VLOOKUP(A3,Отношения!A:E,4,0)</f>
+        <f>VLOOKUP(A3,'Отношения'!A:E,4,0)</f>
       </c>
       <c r="G3" s="0">
-        <f>VLOOKUP(A3,Отношения!A:E,5,0)</f>
+        <f>VLOOKUP(A3,'Отношения'!A:E,5,0)</f>
       </c>
       <c r="H3" t="s" s="0">
         <v>111</v>
       </c>
       <c r="I3" s="0">
-        <f>VLOOKUP(B3&amp;"."&amp;H3,Поля таблиц!A:G,7,0)</f>
+        <f>VLOOKUP(B3&amp;"."&amp;H3,'Поля таблиц'!A:G,7,0)</f>
       </c>
       <c r="J3" t="s" s="0">
         <v>81</v>
       </c>
       <c r="K3" s="0">
-        <f>VLOOKUP(D3&amp;"."&amp;J3,Поля таблиц!A:G,7,0)</f>
+        <f>VLOOKUP(D3&amp;"."&amp;J3,'Поля таблиц'!A:G,7,0)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>